<commit_message>
generation of projects is constrained by geographical space + implementation of municipality groups for positive and negative externalities
</commit_message>
<xml_diff>
--- a/data/municipality_groups.xlsx
+++ b/data/municipality_groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frac1\Documents\GitHub\SEN9120-Regional energy transition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191DBEC3-D58B-4808-B754-4BB025B749B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4D0B29-69EB-4B69-A24B-3A95E83FC3AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-768" yWindow="1308" windowWidth="17508" windowHeight="10728" xr2:uid="{A8E541C3-C1C6-4ED0-BB72-2710B72368FC}"/>
+    <workbookView xWindow="2304" yWindow="2232" windowWidth="17508" windowHeight="10728" xr2:uid="{A8E541C3-C1C6-4ED0-BB72-2710B72368FC}"/>
   </bookViews>
   <sheets>
     <sheet name="municipality_groups" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="29">
   <si>
     <t>Albrandswaard</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Lansingerland</t>
   </si>
   <si>
-    <t>Leidschendam</t>
-  </si>
-  <si>
     <t>Maassluis</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Pijnacker-Nootdorp</t>
   </si>
   <si>
-    <t>Ridderkerk</t>
-  </si>
-  <si>
     <t>Rotterdam</t>
   </si>
   <si>
@@ -124,6 +118,9 @@
   </si>
   <si>
     <t>municipality_5</t>
+  </si>
+  <si>
+    <t>Leidschendam-Voorburg</t>
   </si>
 </sst>
 </file>
@@ -481,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DCF4CD-8B28-469A-8951-DF820C786F79}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,50 +493,50 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -550,10 +547,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -564,21 +561,21 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -587,68 +584,65 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -656,49 +650,52 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -706,43 +703,40 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -750,115 +744,118 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
         <v>3</v>
@@ -866,191 +863,191 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
       </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
         <v>3</v>
@@ -1058,99 +1055,85 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>21</v>
-      </c>
-      <c r="B57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change of the name of The Hague to the csv files
</commit_message>
<xml_diff>
--- a/data/municipality_groups.xlsx
+++ b/data/municipality_groups.xlsx
@@ -1,40 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frac1\Documents\GitHub\SEN9120-Regional energy transition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4D0B29-69EB-4B69-A24B-3A95E83FC3AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C01D0C76-1CF8-414F-8E38-5B0015D15281}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2232" windowWidth="17508" windowHeight="10728" xr2:uid="{A8E541C3-C1C6-4ED0-BB72-2710B72368FC}"/>
+    <workbookView xWindow="5676" yWindow="1572" windowWidth="16788" windowHeight="10728"/>
   </bookViews>
   <sheets>
     <sheet name="municipality_groups" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="35">
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>municipality_1</t>
+  </si>
+  <si>
+    <t>municipality_2</t>
+  </si>
+  <si>
+    <t>municipality_3</t>
+  </si>
+  <si>
+    <t>municipality_4</t>
+  </si>
+  <si>
+    <t>municipality_5</t>
+  </si>
+  <si>
+    <t>offshore-small</t>
+  </si>
+  <si>
+    <t>Westvoorne</t>
+  </si>
+  <si>
+    <t>Rotterdam</t>
+  </si>
+  <si>
+    <t>Westland</t>
+  </si>
+  <si>
+    <t>s-Gravenhage</t>
+  </si>
+  <si>
+    <t>Wassenaar</t>
+  </si>
+  <si>
+    <t>offshore-medium</t>
+  </si>
+  <si>
+    <t>offshore-large</t>
+  </si>
+  <si>
+    <t>onshore-large</t>
+  </si>
+  <si>
+    <t>Brielle</t>
+  </si>
+  <si>
+    <t>Hellevoetsluis</t>
+  </si>
+  <si>
+    <t>Nissewaard</t>
+  </si>
   <si>
     <t>Albrandswaard</t>
   </si>
@@ -42,92 +82,56 @@
     <t>Barendrecht</t>
   </si>
   <si>
-    <t>Brielle</t>
+    <t>Midden-Delfland</t>
+  </si>
+  <si>
+    <t>Vlaardingen</t>
+  </si>
+  <si>
+    <t>Maassluis</t>
+  </si>
+  <si>
+    <t>Schiedam</t>
+  </si>
+  <si>
+    <t>Leidschendam-Voorburg</t>
+  </si>
+  <si>
+    <t>Zoetermeer</t>
+  </si>
+  <si>
+    <t>Pijnacker-Nootdorp</t>
+  </si>
+  <si>
+    <t>Lansingerland</t>
+  </si>
+  <si>
+    <t>onshore-medium</t>
   </si>
   <si>
     <t>Delft</t>
   </si>
   <si>
-    <t>The Hague</t>
-  </si>
-  <si>
-    <t>Hellevoetsluis</t>
-  </si>
-  <si>
-    <t>Lansingerland</t>
-  </si>
-  <si>
-    <t>Maassluis</t>
-  </si>
-  <si>
-    <t>Midden-Delfland</t>
-  </si>
-  <si>
-    <t>Nissewaard</t>
-  </si>
-  <si>
-    <t>Pijnacker-Nootdorp</t>
-  </si>
-  <si>
-    <t>Rotterdam</t>
-  </si>
-  <si>
-    <t>Schiedam</t>
-  </si>
-  <si>
-    <t>Vlaardingen</t>
-  </si>
-  <si>
-    <t>Wassenaar</t>
-  </si>
-  <si>
-    <t>Westland</t>
-  </si>
-  <si>
-    <t>Westvoorne</t>
-  </si>
-  <si>
-    <t>Zoetermeer</t>
-  </si>
-  <si>
-    <t>offshore-wind</t>
-  </si>
-  <si>
     <t>onshore-small</t>
   </si>
   <si>
-    <t>onshore-medium</t>
-  </si>
-  <si>
-    <t>onshore-large</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>municipality_1</t>
-  </si>
-  <si>
-    <t>municipality_2</t>
-  </si>
-  <si>
-    <t>municipality_3</t>
-  </si>
-  <si>
-    <t>municipality_4</t>
-  </si>
-  <si>
-    <t>municipality_5</t>
-  </si>
-  <si>
-    <t>Leidschendam-Voorburg</t>
+    <t>Ridderkerk</t>
+  </si>
+  <si>
+    <t>Capelle aan den IJssel</t>
+  </si>
+  <si>
+    <t>Krimpen aan den IJssel</t>
+  </si>
+  <si>
+    <t>Rijswijk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,21 +140,315 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -158,15 +456,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -477,667 +965,772 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DCF4CD-8B28-469A-8951-DF820C786F79}">
-  <dimension ref="A1:F57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>2</v>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>25</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
         <v>20</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
         <v>20</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
         <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>